<commit_message>
Corrects issue in "Modelling" column. Readme modified.
</commit_message>
<xml_diff>
--- a/Species_list_v4.xlsx
+++ b/Species_list_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\R-dev\OneSTOP_Data\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15BAF99-5313-493E-BA92-A0A2709CD577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F793B48-2C6D-4B66-86B2-92099E85BF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{97DD50A9-AF4B-4AB0-83AD-BDD62E1A22CA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="523">
   <si>
     <t>Synonyms</t>
   </si>
@@ -2088,7 +2088,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="K155" sqref="K155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7197,6 +7197,9 @@
       <c r="I116" s="1" t="s">
         <v>461</v>
       </c>
+      <c r="M116" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N116" s="5" t="s">
         <v>387</v>
       </c>
@@ -7226,6 +7229,9 @@
       <c r="I117" s="1" t="s">
         <v>462</v>
       </c>
+      <c r="M117" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N117" s="5" t="s">
         <v>387</v>
       </c>
@@ -7255,6 +7261,9 @@
       <c r="I118" s="1" t="s">
         <v>463</v>
       </c>
+      <c r="M118" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N118" s="5" t="s">
         <v>387</v>
       </c>
@@ -7284,6 +7293,9 @@
       <c r="I119" s="1" t="s">
         <v>464</v>
       </c>
+      <c r="M119" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N119" s="5" t="s">
         <v>387</v>
       </c>
@@ -7313,6 +7325,9 @@
       <c r="I120" s="1" t="s">
         <v>465</v>
       </c>
+      <c r="M120" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N120" s="5" t="s">
         <v>387</v>
       </c>
@@ -7342,6 +7357,9 @@
       <c r="I121" s="1" t="s">
         <v>466</v>
       </c>
+      <c r="M121" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N121" s="5" t="s">
         <v>387</v>
       </c>
@@ -7371,6 +7389,9 @@
       <c r="I122" s="1" t="s">
         <v>467</v>
       </c>
+      <c r="M122" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N122" s="5" t="s">
         <v>387</v>
       </c>
@@ -7400,6 +7421,9 @@
       <c r="I123" s="1" t="s">
         <v>468</v>
       </c>
+      <c r="M123" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N123" s="5" t="s">
         <v>387</v>
       </c>
@@ -7429,6 +7453,9 @@
       <c r="I124" s="1" t="s">
         <v>469</v>
       </c>
+      <c r="M124" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N124" s="5" t="s">
         <v>387</v>
       </c>
@@ -7458,6 +7485,9 @@
       <c r="I125" s="1" t="s">
         <v>470</v>
       </c>
+      <c r="M125" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N125" s="5" t="s">
         <v>387</v>
       </c>
@@ -7487,6 +7517,9 @@
       <c r="I126" s="1" t="s">
         <v>446</v>
       </c>
+      <c r="M126" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N126" s="5" t="s">
         <v>387</v>
       </c>
@@ -7516,6 +7549,9 @@
       <c r="I127" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="M127" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N127" s="5" t="s">
         <v>387</v>
       </c>
@@ -7545,6 +7581,9 @@
       <c r="I128" s="1" t="s">
         <v>448</v>
       </c>
+      <c r="M128" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N128" s="5" t="s">
         <v>387</v>
       </c>
@@ -7574,6 +7613,9 @@
       <c r="I129" s="1" t="s">
         <v>449</v>
       </c>
+      <c r="M129" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N129" s="5" t="s">
         <v>387</v>
       </c>
@@ -7603,6 +7645,9 @@
       <c r="I130" s="1" t="s">
         <v>450</v>
       </c>
+      <c r="M130" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N130" s="5" t="s">
         <v>387</v>
       </c>
@@ -7632,6 +7677,9 @@
       <c r="I131" s="1" t="s">
         <v>451</v>
       </c>
+      <c r="M131" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N131" s="5" t="s">
         <v>387</v>
       </c>
@@ -7661,6 +7709,9 @@
       <c r="I132" s="1" t="s">
         <v>452</v>
       </c>
+      <c r="M132" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N132" s="5" t="s">
         <v>387</v>
       </c>
@@ -7690,6 +7741,9 @@
       <c r="I133" s="1" t="s">
         <v>453</v>
       </c>
+      <c r="M133" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N133" s="5" t="s">
         <v>387</v>
       </c>
@@ -7719,6 +7773,9 @@
       <c r="I134" s="1" t="s">
         <v>414</v>
       </c>
+      <c r="M134" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N134" s="5" t="s">
         <v>387</v>
       </c>
@@ -7748,6 +7805,9 @@
       <c r="I135" s="1" t="s">
         <v>454</v>
       </c>
+      <c r="M135" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N135" s="5" t="s">
         <v>387</v>
       </c>
@@ -7777,6 +7837,9 @@
       <c r="I136" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="M136" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N136" s="5" t="s">
         <v>387</v>
       </c>
@@ -7806,6 +7869,9 @@
       <c r="I137" s="1" t="s">
         <v>472</v>
       </c>
+      <c r="M137" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N137" s="5" t="s">
         <v>387</v>
       </c>
@@ -7835,6 +7901,9 @@
       <c r="I138" s="1" t="s">
         <v>473</v>
       </c>
+      <c r="M138" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N138" s="5" t="s">
         <v>387</v>
       </c>
@@ -7864,6 +7933,9 @@
       <c r="I139" s="1" t="s">
         <v>474</v>
       </c>
+      <c r="M139" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N139" s="5" t="s">
         <v>387</v>
       </c>
@@ -7893,6 +7965,9 @@
       <c r="I140" s="1" t="s">
         <v>475</v>
       </c>
+      <c r="M140" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N140" s="5" t="s">
         <v>387</v>
       </c>
@@ -7922,6 +7997,9 @@
       <c r="I141" s="1" t="s">
         <v>476</v>
       </c>
+      <c r="M141" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N141" s="5" t="s">
         <v>387</v>
       </c>
@@ -7951,6 +8029,9 @@
       <c r="I142" s="1" t="s">
         <v>477</v>
       </c>
+      <c r="M142" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N142" s="5" t="s">
         <v>387</v>
       </c>
@@ -7980,6 +8061,9 @@
       <c r="I143" s="1" t="s">
         <v>478</v>
       </c>
+      <c r="M143" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N143" s="5" t="s">
         <v>387</v>
       </c>
@@ -8009,6 +8093,9 @@
       <c r="I144" s="1" t="s">
         <v>479</v>
       </c>
+      <c r="M144" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N144" s="5" t="s">
         <v>387</v>
       </c>
@@ -8038,6 +8125,9 @@
       <c r="I145" s="1" t="s">
         <v>480</v>
       </c>
+      <c r="M145" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N145" s="5" t="s">
         <v>387</v>
       </c>
@@ -8067,6 +8157,9 @@
       <c r="I146" s="1" t="s">
         <v>499</v>
       </c>
+      <c r="M146" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N146" s="5" t="s">
         <v>387</v>
       </c>
@@ -8096,6 +8189,9 @@
       <c r="I147" s="1" t="s">
         <v>481</v>
       </c>
+      <c r="M147" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N147" s="5" t="s">
         <v>387</v>
       </c>
@@ -8125,6 +8221,9 @@
       <c r="I148" s="1" t="s">
         <v>482</v>
       </c>
+      <c r="M148" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N148" s="5" t="s">
         <v>387</v>
       </c>
@@ -8154,6 +8253,9 @@
       <c r="I149" s="1" t="s">
         <v>483</v>
       </c>
+      <c r="M149" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N149" s="5" t="s">
         <v>387</v>
       </c>
@@ -8183,6 +8285,9 @@
       <c r="I150" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="M150" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N150" s="5" t="s">
         <v>387</v>
       </c>
@@ -8212,6 +8317,9 @@
       <c r="I151" s="1" t="s">
         <v>484</v>
       </c>
+      <c r="M151" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N151" s="5" t="s">
         <v>387</v>
       </c>
@@ -8241,6 +8349,9 @@
       <c r="I152" s="1" t="s">
         <v>485</v>
       </c>
+      <c r="M152" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N152" s="5" t="s">
         <v>387</v>
       </c>
@@ -8270,6 +8381,9 @@
       <c r="I153" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="M153" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N153" s="5" t="s">
         <v>387</v>
       </c>
@@ -8299,6 +8413,9 @@
       <c r="I154" s="1" t="s">
         <v>487</v>
       </c>
+      <c r="M154" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N154" s="5" t="s">
         <v>387</v>
       </c>
@@ -8328,6 +8445,9 @@
       <c r="I155" s="1" t="s">
         <v>488</v>
       </c>
+      <c r="M155" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N155" s="5" t="s">
         <v>387</v>
       </c>
@@ -8357,6 +8477,9 @@
       <c r="I156" s="1" t="s">
         <v>489</v>
       </c>
+      <c r="M156" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N156" s="5" t="s">
         <v>387</v>
       </c>
@@ -8386,6 +8509,9 @@
       <c r="I157" s="1" t="s">
         <v>490</v>
       </c>
+      <c r="M157" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N157" s="5" t="s">
         <v>387</v>
       </c>
@@ -8415,6 +8541,9 @@
       <c r="I158" s="1" t="s">
         <v>491</v>
       </c>
+      <c r="M158" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N158" s="5" t="s">
         <v>387</v>
       </c>
@@ -8444,6 +8573,9 @@
       <c r="I159" s="1" t="s">
         <v>492</v>
       </c>
+      <c r="M159" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N159" s="5" t="s">
         <v>387</v>
       </c>
@@ -8473,6 +8605,9 @@
       <c r="I160" s="1" t="s">
         <v>493</v>
       </c>
+      <c r="M160" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N160" s="5" t="s">
         <v>387</v>
       </c>
@@ -8502,6 +8637,9 @@
       <c r="I161" s="1" t="s">
         <v>494</v>
       </c>
+      <c r="M161" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N161" s="5" t="s">
         <v>387</v>
       </c>
@@ -8531,6 +8669,9 @@
       <c r="I162" s="1" t="s">
         <v>495</v>
       </c>
+      <c r="M162" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N162" s="5" t="s">
         <v>387</v>
       </c>
@@ -8560,6 +8701,9 @@
       <c r="I163" s="1" t="s">
         <v>496</v>
       </c>
+      <c r="M163" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N163" s="5" t="s">
         <v>387</v>
       </c>
@@ -8589,6 +8733,9 @@
       <c r="I164" s="1" t="s">
         <v>497</v>
       </c>
+      <c r="M164" s="5" t="s">
+        <v>387</v>
+      </c>
       <c r="N164" s="5" t="s">
         <v>387</v>
       </c>
@@ -8623,7 +8770,9 @@
       <c r="J165" s="8"/>
       <c r="K165" s="8"/>
       <c r="L165" s="8"/>
-      <c r="M165" s="8"/>
+      <c r="M165" s="8" t="s">
+        <v>387</v>
+      </c>
       <c r="N165" s="8" t="s">
         <v>387</v>
       </c>

</xml_diff>